<commit_message>
orders (werkt nog niet zoals t hoort)
</commit_message>
<xml_diff>
--- a/dev/gouden_draak/public/salesreport.xlsx
+++ b/dev/gouden_draak/public/salesreport.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>2024-08-23</t>
+  </si>
+  <si>
+    <t>Orders</t>
   </si>
 </sst>
 </file>
@@ -372,7 +375,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -414,6 +417,11 @@
         <v>790.0</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>